<commit_message>
Cleaned version and validated
This script is giving same CoR and CoM for a rectangular box which is correct.
</commit_message>
<xml_diff>
--- a/shearwall_data_R3.xlsx
+++ b/shearwall_data_R3.xlsx
@@ -737,7 +737,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="ShearWallPlot"/>
+        <xdr:cNvPr id="5" name="ShearWallPlot"/>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
@@ -2192,7 +2192,7 @@
   <dimension ref="B1:AM61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q38" sqref="Q38"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="M3" s="44">
         <f ca="1">NOW()</f>
-        <v>45668.38619409722</v>
+        <v>45669.347327199073</v>
       </c>
       <c r="N3" s="44"/>
       <c r="O3" s="15"/>
@@ -2343,7 +2343,7 @@
         <v>12</v>
       </c>
       <c r="J10" s="38">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="K10" s="15" t="s">
         <v>14</v>
@@ -2453,7 +2453,7 @@
         <v>12</v>
       </c>
       <c r="J13" s="31">
-        <v>40.237418469837962</v>
+        <v>25</v>
       </c>
       <c r="K13" s="15" t="s">
         <v>14</v>
@@ -2465,7 +2465,7 @@
         <v>12</v>
       </c>
       <c r="N13" s="31">
-        <v>8.3340101015906072</v>
+        <v>0</v>
       </c>
       <c r="O13" s="15" t="s">
         <v>14</v>
@@ -2515,7 +2515,7 @@
         <v>12</v>
       </c>
       <c r="J14" s="31">
-        <v>24.976167621065173</v>
+        <v>25</v>
       </c>
       <c r="K14" s="15" t="s">
         <v>14</v>
@@ -2527,7 +2527,7 @@
         <v>12</v>
       </c>
       <c r="N14" s="31">
-        <v>1.3804229402141104</v>
+        <v>0</v>
       </c>
       <c r="O14" s="15" t="s">
         <v>14</v>
@@ -2615,7 +2615,7 @@
         <v>12</v>
       </c>
       <c r="J16" s="31">
-        <v>48.571428571428569</v>
+        <v>25</v>
       </c>
       <c r="K16" s="15" t="s">
         <v>14</v>
@@ -2665,7 +2665,7 @@
         <v>12</v>
       </c>
       <c r="J17" s="31">
-        <v>23.595744680851062</v>
+        <v>25</v>
       </c>
       <c r="K17" s="15" t="s">
         <v>14</v>
@@ -2753,7 +2753,7 @@
         <v>12</v>
       </c>
       <c r="J19" s="40">
-        <v>150519.25941332532</v>
+        <v>62500</v>
       </c>
       <c r="K19" s="15"/>
       <c r="AD19" s="13" t="s">
@@ -2801,7 +2801,7 @@
         <v>12</v>
       </c>
       <c r="J20" s="40">
-        <v>43785.788327162234</v>
+        <v>62500</v>
       </c>
       <c r="K20" s="15"/>
       <c r="AD20" s="13" t="s">
@@ -2888,7 +2888,7 @@
       </c>
       <c r="J22" s="39">
         <f>J10*J11</f>
-        <v>4000</v>
+        <v>2500</v>
       </c>
       <c r="K22" s="15" t="s">
         <v>85</v>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="J23" s="39">
         <f>2.39*J22</f>
-        <v>9560</v>
+        <v>5975</v>
       </c>
       <c r="K23" s="11" t="s">
         <v>88</v>
@@ -3150,16 +3150,16 @@
         <v>0</v>
       </c>
       <c r="I29" s="28">
-        <v>40.237418469837962</v>
+        <v>25</v>
       </c>
       <c r="J29" s="32">
-        <v>0.53191489361702127</v>
+        <v>0.5</v>
       </c>
       <c r="K29" s="28">
-        <v>16.334010101590607</v>
+        <v>5</v>
       </c>
       <c r="L29" s="11">
-        <v>0.53405348604043179</v>
+        <v>0.502</v>
       </c>
       <c r="O29" s="13" t="s">
         <v>53</v>
@@ -3168,28 +3168,28 @@
         <v>1</v>
       </c>
       <c r="Q29" s="21">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="R29" s="13">
         <v>3.2</v>
       </c>
       <c r="S29" s="21">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="T29" s="21">
         <v>0</v>
       </c>
       <c r="U29" s="28">
-        <v>24.976167621065173</v>
+        <v>25</v>
       </c>
       <c r="V29" s="11">
-        <v>0.2857142857142857</v>
+        <v>0.5</v>
       </c>
       <c r="W29" s="29">
-        <v>6.3804229402141104</v>
+        <v>5</v>
       </c>
       <c r="X29" s="11">
-        <v>0.28856637181062889</v>
+        <v>0.502</v>
       </c>
       <c r="AC29" s="11">
         <v>0</v>
@@ -3218,28 +3218,28 @@
         <v>2</v>
       </c>
       <c r="E30" s="21">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F30" s="13">
         <v>3.2</v>
       </c>
       <c r="G30" s="21">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H30" s="21">
         <v>0</v>
       </c>
       <c r="I30" s="28">
-        <v>39.762581530162038</v>
+        <v>25</v>
       </c>
       <c r="J30" s="32">
-        <v>0.46808510638297873</v>
+        <v>0.5</v>
       </c>
       <c r="K30" s="28">
-        <v>16.334010101590607</v>
+        <v>5</v>
       </c>
       <c r="L30" s="11">
-        <v>0.47019846153421418</v>
+        <v>0.502</v>
       </c>
       <c r="O30" s="13" t="s">
         <v>54</v>
@@ -3254,22 +3254,22 @@
         <v>3.2</v>
       </c>
       <c r="S30" s="21">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T30" s="21">
         <v>50</v>
       </c>
       <c r="U30" s="28">
-        <v>25.023832378934827</v>
+        <v>25</v>
       </c>
       <c r="V30" s="11">
-        <v>0.7142857142857143</v>
+        <v>0.5</v>
       </c>
       <c r="W30" s="29">
-        <v>6.3804229402141104</v>
+        <v>5</v>
       </c>
       <c r="X30" s="11">
-        <v>0.71714324333052215</v>
+        <v>0.502</v>
       </c>
       <c r="AC30" s="11">
         <v>1</v>

</xml_diff>

<commit_message>
Added shapely roof diaphragm data
Now I can export roof diaphragm centroid from shapely
</commit_message>
<xml_diff>
--- a/shearwall_data_R3.xlsx
+++ b/shearwall_data_R3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
   <si>
     <t>Wall ID</t>
   </si>
@@ -531,7 +531,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -608,6 +608,15 @@
     <xf numFmtId="15" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,7 +746,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="ShearWallPlot"/>
+        <xdr:cNvPr id="16" name="ShearWallPlot"/>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
@@ -2192,7 +2201,7 @@
   <dimension ref="B1:AM61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2267,7 +2276,7 @@
       </c>
       <c r="M3" s="44">
         <f ca="1">NOW()</f>
-        <v>45669.347327199073</v>
+        <v>45669.785043750002</v>
       </c>
       <c r="N3" s="44"/>
       <c r="O3" s="15"/>
@@ -2348,7 +2357,12 @@
       <c r="K10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="38"/>
+      <c r="L10" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="M10" s="49" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="2:39" x14ac:dyDescent="0.2">
       <c r="D11" s="15" t="s">
@@ -2369,7 +2383,12 @@
       <c r="K11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="38"/>
+      <c r="L11" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="49" t="s">
+        <v>12</v>
+      </c>
       <c r="AD11" s="13" t="s">
         <v>20</v>
       </c>
@@ -2408,6 +2427,7 @@
       <c r="I12" s="27"/>
       <c r="J12" s="30"/>
       <c r="K12" s="24"/>
+      <c r="M12" s="49"/>
       <c r="AD12" s="13" t="s">
         <v>21</v>
       </c>
@@ -2453,7 +2473,7 @@
         <v>12</v>
       </c>
       <c r="J13" s="31">
-        <v>25</v>
+        <v>25.028173166322986</v>
       </c>
       <c r="K13" s="15" t="s">
         <v>14</v>
@@ -2465,7 +2485,7 @@
         <v>12</v>
       </c>
       <c r="N13" s="31">
-        <v>0</v>
+        <v>10.833163282944582</v>
       </c>
       <c r="O13" s="15" t="s">
         <v>14</v>
@@ -2515,7 +2535,7 @@
         <v>12</v>
       </c>
       <c r="J14" s="31">
-        <v>25</v>
+        <v>24.987196142941343</v>
       </c>
       <c r="K14" s="15" t="s">
         <v>14</v>
@@ -2527,7 +2547,7 @@
         <v>12</v>
       </c>
       <c r="N14" s="31">
-        <v>0</v>
+        <v>3.2911080514203412</v>
       </c>
       <c r="O14" s="15" t="s">
         <v>14</v>
@@ -2615,7 +2635,7 @@
         <v>12</v>
       </c>
       <c r="J16" s="31">
-        <v>25</v>
+        <v>35.861336449267569</v>
       </c>
       <c r="K16" s="15" t="s">
         <v>14</v>
@@ -2665,7 +2685,7 @@
         <v>12</v>
       </c>
       <c r="J17" s="31">
-        <v>25</v>
+        <v>21.696088091521002</v>
       </c>
       <c r="K17" s="15" t="s">
         <v>14</v>
@@ -2753,7 +2773,7 @@
         <v>12</v>
       </c>
       <c r="J19" s="40">
-        <v>62500</v>
+        <v>21153.219729859389</v>
       </c>
       <c r="K19" s="15"/>
       <c r="AD19" s="13" t="s">
@@ -2801,7 +2821,7 @@
         <v>12</v>
       </c>
       <c r="J20" s="40">
-        <v>62500</v>
+        <v>7607.6975547618522</v>
       </c>
       <c r="K20" s="15"/>
       <c r="AD20" s="13" t="s">
@@ -3131,65 +3151,65 @@
       </c>
     </row>
     <row r="29" spans="3:39" x14ac:dyDescent="0.2">
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="45">
         <v>1</v>
       </c>
-      <c r="E29" s="21">
-        <v>50</v>
-      </c>
-      <c r="F29" s="13">
-        <v>3.2</v>
-      </c>
-      <c r="G29" s="21">
-        <v>0</v>
-      </c>
-      <c r="H29" s="21">
-        <v>0</v>
+      <c r="E29" s="47">
+        <v>4.6341463414634143</v>
+      </c>
+      <c r="F29" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G29" s="47">
+        <v>2.1036585365853662</v>
+      </c>
+      <c r="H29" s="47">
+        <v>23.658536585365852</v>
       </c>
       <c r="I29" s="28">
-        <v>25</v>
+        <v>22.924514629737619</v>
       </c>
       <c r="J29" s="32">
-        <v>0.5</v>
+        <v>3.9874081846799567E-2</v>
       </c>
       <c r="K29" s="28">
-        <v>5</v>
+        <v>15.833163282944582</v>
       </c>
       <c r="L29" s="11">
-        <v>0.502</v>
-      </c>
-      <c r="O29" s="13" t="s">
+        <v>4.5292763948744055E-2</v>
+      </c>
+      <c r="O29" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="P29" s="13">
+      <c r="P29" s="50">
         <v>1</v>
       </c>
-      <c r="Q29" s="21">
-        <v>50</v>
-      </c>
-      <c r="R29" s="13">
-        <v>3.2</v>
-      </c>
-      <c r="S29" s="21">
-        <v>0</v>
-      </c>
-      <c r="T29" s="21">
-        <v>0</v>
+      <c r="Q29" s="52">
+        <v>5.1524390243902438</v>
+      </c>
+      <c r="R29" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="S29" s="52">
+        <v>12.774390243902401</v>
+      </c>
+      <c r="T29" s="52">
+        <v>18.841463414634145</v>
       </c>
       <c r="U29" s="28">
-        <v>25</v>
+        <v>6.1457327283071983</v>
       </c>
       <c r="V29" s="11">
-        <v>0.5</v>
+        <v>8.272148800783162E-2</v>
       </c>
       <c r="W29" s="29">
-        <v>5</v>
+        <v>8.2911080514203412</v>
       </c>
       <c r="X29" s="11">
-        <v>0.502</v>
+        <v>8.6760642222407633E-2</v>
       </c>
       <c r="AC29" s="11">
         <v>0</v>
@@ -3211,65 +3231,65 @@
       </c>
     </row>
     <row r="30" spans="3:39" x14ac:dyDescent="0.2">
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="45">
         <v>2</v>
       </c>
-      <c r="E30" s="21">
-        <v>50</v>
-      </c>
-      <c r="F30" s="13">
-        <v>3.2</v>
-      </c>
-      <c r="G30" s="21">
-        <v>50</v>
-      </c>
-      <c r="H30" s="21">
-        <v>0</v>
+      <c r="E30" s="47">
+        <v>6.7682926829268295</v>
+      </c>
+      <c r="F30" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G30" s="47">
+        <v>9.7560975609756095</v>
+      </c>
+      <c r="H30" s="47">
+        <v>24.115853658536587</v>
       </c>
       <c r="I30" s="28">
-        <v>25</v>
+        <v>15.272075605347377</v>
       </c>
       <c r="J30" s="32">
-        <v>0.5</v>
+        <v>5.8237145855194114E-2</v>
       </c>
       <c r="K30" s="28">
-        <v>5</v>
+        <v>15.833163282944582</v>
       </c>
       <c r="L30" s="11">
-        <v>0.502</v>
-      </c>
-      <c r="O30" s="13" t="s">
+        <v>6.1847016078352073E-2</v>
+      </c>
+      <c r="O30" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="P30" s="13">
+      <c r="P30" s="50">
         <v>2</v>
       </c>
-      <c r="Q30" s="21">
-        <v>50</v>
-      </c>
-      <c r="R30" s="13">
-        <v>3.2</v>
-      </c>
-      <c r="S30" s="21">
-        <v>0</v>
-      </c>
-      <c r="T30" s="21">
-        <v>50</v>
+      <c r="Q30" s="52">
+        <v>5.7926829268292686</v>
+      </c>
+      <c r="R30" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="S30" s="52">
+        <v>25.2134146341463</v>
+      </c>
+      <c r="T30" s="52">
+        <v>18.841463414634145</v>
       </c>
       <c r="U30" s="28">
-        <v>25</v>
+        <v>6.1457327283071983</v>
       </c>
       <c r="V30" s="11">
-        <v>0.5</v>
+        <v>9.3000489476260398E-2</v>
       </c>
       <c r="W30" s="29">
-        <v>5</v>
+        <v>8.2911080514203412</v>
       </c>
       <c r="X30" s="11">
-        <v>0.502</v>
+        <v>9.7039643690836411E-2</v>
       </c>
       <c r="AC30" s="11">
         <v>1</v>
@@ -3291,23 +3311,66 @@
       </c>
     </row>
     <row r="31" spans="3:39" x14ac:dyDescent="0.2">
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="28"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21"/>
-      <c r="U31" s="28"/>
-      <c r="W31" s="29"/>
+      <c r="C31" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="45">
+        <v>3</v>
+      </c>
+      <c r="E31" s="47">
+        <v>4.0853658536585371</v>
+      </c>
+      <c r="F31" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G31" s="47">
+        <v>9.7560975609756095</v>
+      </c>
+      <c r="H31" s="47">
+        <v>16.371951219512198</v>
+      </c>
+      <c r="I31" s="28">
+        <v>15.272075605347377</v>
+      </c>
+      <c r="J31" s="32">
+        <v>3.5152151101783838E-2</v>
+      </c>
+      <c r="K31" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L31" s="11">
+        <v>3.8762021324941796E-2</v>
+      </c>
+      <c r="O31" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="P31" s="50">
+        <v>3</v>
+      </c>
+      <c r="Q31" s="52">
+        <v>3.8414634146341466</v>
+      </c>
+      <c r="R31" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="S31" s="52">
+        <v>31.6768292682927</v>
+      </c>
+      <c r="T31" s="52">
+        <v>18.841463414634145</v>
+      </c>
+      <c r="U31" s="28">
+        <v>6.1457327283071983</v>
+      </c>
+      <c r="V31" s="11">
+        <v>6.1674008810572688E-2</v>
+      </c>
+      <c r="W31" s="29">
+        <v>8.2911080514203412</v>
+      </c>
+      <c r="X31" s="11">
+        <v>6.5713163025148708E-2</v>
+      </c>
       <c r="AC31" s="11">
         <v>2</v>
       </c>
@@ -3328,23 +3391,66 @@
       </c>
     </row>
     <row r="32" spans="3:39" x14ac:dyDescent="0.2">
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="28"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
-      <c r="U32" s="28"/>
-      <c r="W32" s="29"/>
+      <c r="C32" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="45">
+        <v>4</v>
+      </c>
+      <c r="E32" s="47">
+        <v>4.0853658536585371</v>
+      </c>
+      <c r="F32" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G32" s="47">
+        <v>9.7560975609756095</v>
+      </c>
+      <c r="H32" s="47">
+        <v>16.371951219512198</v>
+      </c>
+      <c r="I32" s="28">
+        <v>15.272075605347377</v>
+      </c>
+      <c r="J32" s="32">
+        <v>3.5152151101783838E-2</v>
+      </c>
+      <c r="K32" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L32" s="11">
+        <v>3.8762021324941796E-2</v>
+      </c>
+      <c r="O32" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="P32" s="50">
+        <v>4</v>
+      </c>
+      <c r="Q32" s="52">
+        <v>4.5731707317073171</v>
+      </c>
+      <c r="R32" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="S32" s="52">
+        <v>37.652439024390198</v>
+      </c>
+      <c r="T32" s="52">
+        <v>18.841463414634145</v>
+      </c>
+      <c r="U32" s="28">
+        <v>6.1457327283071983</v>
+      </c>
+      <c r="V32" s="11">
+        <v>7.3421439060205582E-2</v>
+      </c>
+      <c r="W32" s="29">
+        <v>8.2911080514203412</v>
+      </c>
+      <c r="X32" s="11">
+        <v>7.7460593274781595E-2</v>
+      </c>
       <c r="AC32" s="11">
         <v>3</v>
       </c>
@@ -3365,23 +3471,66 @@
       </c>
     </row>
     <row r="33" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="28"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="13"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="28"/>
-      <c r="W33" s="29"/>
+      <c r="C33" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="45">
+        <v>5</v>
+      </c>
+      <c r="E33" s="47">
+        <v>7.5914634146341466</v>
+      </c>
+      <c r="F33" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G33" s="47">
+        <v>12.652439024390244</v>
+      </c>
+      <c r="H33" s="47">
+        <v>24.527439024390247</v>
+      </c>
+      <c r="I33" s="28">
+        <v>12.375734141932742</v>
+      </c>
+      <c r="J33" s="32">
+        <v>6.5320041972717721E-2</v>
+      </c>
+      <c r="K33" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L33" s="11">
+        <v>6.8245302122231372E-2</v>
+      </c>
+      <c r="O33" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="P33" s="50">
+        <v>5</v>
+      </c>
+      <c r="Q33" s="52">
+        <v>6.6768292682926829</v>
+      </c>
+      <c r="R33" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="S33" s="52">
+        <v>18.978658536585399</v>
+      </c>
+      <c r="T33" s="52">
+        <v>20.54878048780488</v>
+      </c>
+      <c r="U33" s="28">
+        <v>4.4384156551364633</v>
+      </c>
+      <c r="V33" s="11">
+        <v>0.10719530102790015</v>
+      </c>
+      <c r="W33" s="29">
+        <v>8.2911080514203412</v>
+      </c>
+      <c r="X33" s="11">
+        <v>0.11011235682775798</v>
+      </c>
       <c r="AC33" s="11">
         <v>4</v>
       </c>
@@ -3402,23 +3551,66 @@
       </c>
     </row>
     <row r="34" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="28"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="21"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
-      <c r="U34" s="28"/>
-      <c r="W34" s="29"/>
+      <c r="C34" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="45">
+        <v>6</v>
+      </c>
+      <c r="E34" s="47">
+        <v>7.6219512195121952</v>
+      </c>
+      <c r="F34" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G34" s="47">
+        <v>18.902439024390244</v>
+      </c>
+      <c r="H34" s="47">
+        <v>24.390243902439025</v>
+      </c>
+      <c r="I34" s="28">
+        <v>6.1257341419327425</v>
+      </c>
+      <c r="J34" s="32">
+        <v>6.5582371458551933E-2</v>
+      </c>
+      <c r="K34" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L34" s="11">
+        <v>6.7030315133359455E-2</v>
+      </c>
+      <c r="O34" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="P34" s="50">
+        <v>6</v>
+      </c>
+      <c r="Q34" s="52">
+        <v>6.524390243902439</v>
+      </c>
+      <c r="R34" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="S34" s="52">
+        <v>27.408536585365901</v>
+      </c>
+      <c r="T34" s="52">
+        <v>20.54878048780488</v>
+      </c>
+      <c r="U34" s="28">
+        <v>4.4384156551364633</v>
+      </c>
+      <c r="V34" s="11">
+        <v>0.10474791972589328</v>
+      </c>
+      <c r="W34" s="29">
+        <v>8.2911080514203412</v>
+      </c>
+      <c r="X34" s="11">
+        <v>0.10766497552575112</v>
+      </c>
       <c r="AC34" s="11">
         <v>5</v>
       </c>
@@ -3439,23 +3631,66 @@
       </c>
     </row>
     <row r="35" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="28"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="21"/>
-      <c r="T35" s="21"/>
-      <c r="U35" s="28"/>
-      <c r="W35" s="29"/>
+      <c r="C35" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="45">
+        <v>7</v>
+      </c>
+      <c r="E35" s="47">
+        <v>7.6219512195121952</v>
+      </c>
+      <c r="F35" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G35" s="47">
+        <v>18.902439024390244</v>
+      </c>
+      <c r="H35" s="47">
+        <v>14.939024390243903</v>
+      </c>
+      <c r="I35" s="28">
+        <v>6.1257341419327425</v>
+      </c>
+      <c r="J35" s="32">
+        <v>6.5582371458551933E-2</v>
+      </c>
+      <c r="K35" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L35" s="11">
+        <v>6.7030315133359455E-2</v>
+      </c>
+      <c r="O35" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="P35" s="50">
+        <v>7</v>
+      </c>
+      <c r="Q35" s="52">
+        <v>5.8841463414634152</v>
+      </c>
+      <c r="R35" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="S35" s="52">
+        <v>34.954268292682897</v>
+      </c>
+      <c r="T35" s="52">
+        <v>20.54878048780488</v>
+      </c>
+      <c r="U35" s="28">
+        <v>4.4384156551364633</v>
+      </c>
+      <c r="V35" s="11">
+        <v>9.4468918257464521E-2</v>
+      </c>
+      <c r="W35" s="29">
+        <v>8.2911080514203412</v>
+      </c>
+      <c r="X35" s="11">
+        <v>9.7385974057322355E-2</v>
+      </c>
       <c r="AC35" s="11">
         <v>6</v>
       </c>
@@ -3476,23 +3711,66 @@
       </c>
     </row>
     <row r="36" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="28"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="21"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="21"/>
-      <c r="T36" s="21"/>
-      <c r="U36" s="28"/>
-      <c r="W36" s="29"/>
+      <c r="C36" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="45">
+        <v>8</v>
+      </c>
+      <c r="E36" s="47">
+        <v>7.6219512195121952</v>
+      </c>
+      <c r="F36" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G36" s="47">
+        <v>25.152439024390244</v>
+      </c>
+      <c r="H36" s="47">
+        <v>24.390243902439025</v>
+      </c>
+      <c r="I36" s="28">
+        <v>0.12426585806725754</v>
+      </c>
+      <c r="J36" s="32">
+        <v>6.5582371458551933E-2</v>
+      </c>
+      <c r="K36" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L36" s="11">
+        <v>6.5611744258450538E-2</v>
+      </c>
+      <c r="O36" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="P36" s="50">
+        <v>8</v>
+      </c>
+      <c r="Q36" s="52">
+        <v>6.5853658536585371</v>
+      </c>
+      <c r="R36" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="S36" s="52">
+        <v>45.975609756097597</v>
+      </c>
+      <c r="T36" s="52">
+        <v>19.969512195121954</v>
+      </c>
+      <c r="U36" s="28">
+        <v>5.0176839478193891</v>
+      </c>
+      <c r="V36" s="11">
+        <v>0.10572687224669604</v>
+      </c>
+      <c r="W36" s="29">
+        <v>8.2911080514203412</v>
+      </c>
+      <c r="X36" s="11">
+        <v>0.1090246400086904</v>
+      </c>
       <c r="AC36" s="11">
         <v>7</v>
       </c>
@@ -3513,23 +3791,66 @@
       </c>
     </row>
     <row r="37" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="28"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-      <c r="Q37" s="21"/>
-      <c r="R37" s="13"/>
-      <c r="S37" s="21"/>
-      <c r="T37" s="21"/>
-      <c r="U37" s="28"/>
-      <c r="W37" s="29"/>
+      <c r="C37" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="45">
+        <v>9</v>
+      </c>
+      <c r="E37" s="47">
+        <v>7.6219512195121952</v>
+      </c>
+      <c r="F37" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G37" s="47">
+        <v>25.457317073170735</v>
+      </c>
+      <c r="H37" s="47">
+        <v>14.939024390243903</v>
+      </c>
+      <c r="I37" s="28">
+        <v>0.42914390684774872</v>
+      </c>
+      <c r="J37" s="32">
+        <v>6.5582371458551933E-2</v>
+      </c>
+      <c r="K37" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L37" s="11">
+        <v>6.5683808476728889E-2</v>
+      </c>
+      <c r="O37" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="P37" s="50">
+        <v>9</v>
+      </c>
+      <c r="Q37" s="52">
+        <v>7.8963414634146343</v>
+      </c>
+      <c r="R37" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="S37" s="52">
+        <v>45.716463414634099</v>
+      </c>
+      <c r="T37" s="52">
+        <v>10.975609756097562</v>
+      </c>
+      <c r="U37" s="28">
+        <v>14.011586386843781</v>
+      </c>
+      <c r="V37" s="11">
+        <v>0.12677435144395496</v>
+      </c>
+      <c r="W37" s="29">
+        <v>8.2911080514203412</v>
+      </c>
+      <c r="X37" s="11">
+        <v>0.13598317335491117</v>
+      </c>
       <c r="AC37" s="11">
         <v>8</v>
       </c>
@@ -3550,23 +3871,66 @@
       </c>
     </row>
     <row r="38" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="28"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13"/>
-      <c r="Q38" s="21"/>
-      <c r="R38" s="13"/>
-      <c r="S38" s="21"/>
-      <c r="T38" s="21"/>
-      <c r="U38" s="28"/>
-      <c r="W38" s="29"/>
+      <c r="C38" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="45">
+        <v>10</v>
+      </c>
+      <c r="E38" s="47">
+        <v>4.5731707317073171</v>
+      </c>
+      <c r="F38" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G38" s="47">
+        <v>31.097560975609756</v>
+      </c>
+      <c r="H38" s="47">
+        <v>25.762195121951223</v>
+      </c>
+      <c r="I38" s="28">
+        <v>6.0693878092867699</v>
+      </c>
+      <c r="J38" s="32">
+        <v>3.9349422875131157E-2</v>
+      </c>
+      <c r="K38" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L38" s="11">
+        <v>4.078404793145754E-2</v>
+      </c>
+      <c r="O38" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="P38" s="50">
+        <v>10</v>
+      </c>
+      <c r="Q38" s="52">
+        <v>2.1951219512195124</v>
+      </c>
+      <c r="R38" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="S38" s="52">
+        <v>34.939024390243901</v>
+      </c>
+      <c r="T38" s="52">
+        <v>2.3780487804878048</v>
+      </c>
+      <c r="U38" s="28">
+        <v>22.609147362453538</v>
+      </c>
+      <c r="V38" s="11">
+        <v>3.5242290748898682E-2</v>
+      </c>
+      <c r="W38" s="29">
+        <v>8.2911080514203412</v>
+      </c>
+      <c r="X38" s="11">
+        <v>5.0101679676828589E-2</v>
+      </c>
       <c r="AC38" s="11">
         <v>9</v>
       </c>
@@ -3587,23 +3951,66 @@
       </c>
     </row>
     <row r="39" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="28"/>
-      <c r="O39" s="13"/>
-      <c r="P39" s="13"/>
-      <c r="Q39" s="21"/>
-      <c r="R39" s="13"/>
-      <c r="S39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="28"/>
-      <c r="W39" s="29"/>
+      <c r="C39" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="45">
+        <v>11</v>
+      </c>
+      <c r="E39" s="47">
+        <v>7.6219512195121952</v>
+      </c>
+      <c r="F39" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G39" s="47">
+        <v>34.451219512195124</v>
+      </c>
+      <c r="H39" s="47">
+        <v>24.390243902439025</v>
+      </c>
+      <c r="I39" s="28">
+        <v>9.4230463458721374</v>
+      </c>
+      <c r="J39" s="32">
+        <v>6.5582371458551933E-2</v>
+      </c>
+      <c r="K39" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L39" s="11">
+        <v>6.7809702915940143E-2</v>
+      </c>
+      <c r="O39" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="P39" s="50">
+        <v>11</v>
+      </c>
+      <c r="Q39" s="52">
+        <v>2.1036585365853662</v>
+      </c>
+      <c r="R39" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="S39" s="52">
+        <v>37.637195121951201</v>
+      </c>
+      <c r="T39" s="52">
+        <v>2.3780487804878048</v>
+      </c>
+      <c r="U39" s="28">
+        <v>22.609147362453538</v>
+      </c>
+      <c r="V39" s="11">
+        <v>3.3773861967694573E-2</v>
+      </c>
+      <c r="W39" s="29">
+        <v>8.2911080514203412</v>
+      </c>
+      <c r="X39" s="11">
+        <v>4.863325089562448E-2</v>
+      </c>
       <c r="AC39" s="11">
         <v>10</v>
       </c>
@@ -3624,26 +4031,68 @@
       </c>
     </row>
     <row r="40" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C40" s="13"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="41"/>
-      <c r="L40" s="12"/>
+      <c r="C40" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="46">
+        <v>12</v>
+      </c>
+      <c r="E40" s="48">
+        <v>4.4207317073170733</v>
+      </c>
+      <c r="F40" s="46">
+        <v>3.2</v>
+      </c>
+      <c r="G40" s="48">
+        <v>37.195121951219512</v>
+      </c>
+      <c r="H40" s="48">
+        <v>14.710365853658537</v>
+      </c>
+      <c r="I40" s="28">
+        <v>12.166948784896526</v>
+      </c>
+      <c r="J40" s="33">
+        <v>3.8037775445960119E-2</v>
+      </c>
+      <c r="K40" s="41">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L40" s="12">
+        <v>4.0913684867853455E-2</v>
+      </c>
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="22"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="22"/>
-      <c r="T40" s="22"/>
-      <c r="U40" s="28"/>
-      <c r="W40" s="29"/>
+      <c r="O40" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="P40" s="51">
+        <v>12</v>
+      </c>
+      <c r="Q40" s="53">
+        <v>1.9817073170731709</v>
+      </c>
+      <c r="R40" s="51">
+        <v>3.2</v>
+      </c>
+      <c r="S40" s="53">
+        <v>41.539634146341498</v>
+      </c>
+      <c r="T40" s="53">
+        <v>2.3780487804878048</v>
+      </c>
+      <c r="U40" s="28">
+        <v>22.609147362453538</v>
+      </c>
+      <c r="V40" s="11">
+        <v>3.1815956926089087E-2</v>
+      </c>
+      <c r="W40" s="29">
+        <v>8.2911080514203412</v>
+      </c>
+      <c r="X40" s="11">
+        <v>4.6675345854018994E-2</v>
+      </c>
       <c r="AC40" s="11">
         <v>11</v>
       </c>
@@ -3664,26 +4113,68 @@
       </c>
     </row>
     <row r="41" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C41" s="13"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="41"/>
-      <c r="L41" s="12"/>
+      <c r="C41" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="46">
+        <v>13</v>
+      </c>
+      <c r="E41" s="48">
+        <v>7.6219512195121952</v>
+      </c>
+      <c r="F41" s="46">
+        <v>3.2</v>
+      </c>
+      <c r="G41" s="48">
+        <v>40.701219512195124</v>
+      </c>
+      <c r="H41" s="48">
+        <v>24.390243902439025</v>
+      </c>
+      <c r="I41" s="28">
+        <v>15.673046345872137</v>
+      </c>
+      <c r="J41" s="33">
+        <v>6.5582371458551933E-2</v>
+      </c>
+      <c r="K41" s="41">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L41" s="12">
+        <v>6.9287019390646271E-2</v>
+      </c>
       <c r="M41" s="12"/>
       <c r="N41" s="12"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="22"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="22"/>
-      <c r="T41" s="22"/>
-      <c r="U41" s="28"/>
-      <c r="W41" s="29"/>
+      <c r="O41" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="P41" s="51">
+        <v>13</v>
+      </c>
+      <c r="Q41" s="53">
+        <v>3.0792682926829271</v>
+      </c>
+      <c r="R41" s="51">
+        <v>3.2</v>
+      </c>
+      <c r="S41" s="53">
+        <v>46.0518292682927</v>
+      </c>
+      <c r="T41" s="53">
+        <v>2.3780487804878048</v>
+      </c>
+      <c r="U41" s="28">
+        <v>22.609147362453538</v>
+      </c>
+      <c r="V41" s="11">
+        <v>4.9437102300538424E-2</v>
+      </c>
+      <c r="W41" s="29">
+        <v>8.2911080514203412</v>
+      </c>
+      <c r="X41" s="11">
+        <v>6.4296491228468325E-2</v>
+      </c>
       <c r="AC41" s="11">
         <v>12</v>
       </c>
@@ -3704,16 +4195,36 @@
       </c>
     </row>
     <row r="42" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="33"/>
-      <c r="K42" s="41"/>
-      <c r="L42" s="12"/>
+      <c r="C42" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="46">
+        <v>14</v>
+      </c>
+      <c r="E42" s="48">
+        <v>7.6219512195121952</v>
+      </c>
+      <c r="F42" s="46">
+        <v>3.2</v>
+      </c>
+      <c r="G42" s="48">
+        <v>40.701219512195124</v>
+      </c>
+      <c r="H42" s="48">
+        <v>24.390243902439025</v>
+      </c>
+      <c r="I42" s="28">
+        <v>15.673046345872137</v>
+      </c>
+      <c r="J42" s="33">
+        <v>6.5582371458551933E-2</v>
+      </c>
+      <c r="K42" s="41">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L42" s="12">
+        <v>6.9287019390646271E-2</v>
+      </c>
       <c r="M42" s="12"/>
       <c r="N42" s="12"/>
       <c r="O42" s="14"/>
@@ -3743,15 +4254,36 @@
       </c>
     </row>
     <row r="43" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C43" s="13"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="28"/>
+      <c r="C43" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="46">
+        <v>15</v>
+      </c>
+      <c r="E43" s="47">
+        <v>2.8963414634146343</v>
+      </c>
+      <c r="F43" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G43" s="47">
+        <v>37.804878048780488</v>
+      </c>
+      <c r="H43" s="47">
+        <v>3.8871951219512195</v>
+      </c>
+      <c r="I43" s="28">
+        <v>12.776704882457501</v>
+      </c>
+      <c r="J43" s="32">
+        <v>2.4921301154249734E-2</v>
+      </c>
+      <c r="K43" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L43" s="11">
+        <v>2.7941339012699767E-2</v>
+      </c>
       <c r="O43" s="13"/>
       <c r="P43" s="13"/>
       <c r="Q43" s="13"/>
@@ -3779,15 +4311,36 @@
       </c>
     </row>
     <row r="44" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C44" s="13"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="28"/>
+      <c r="C44" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="46">
+        <v>16</v>
+      </c>
+      <c r="E44" s="47">
+        <v>6.8292682926829267</v>
+      </c>
+      <c r="F44" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G44" s="47">
+        <v>41.768292682926834</v>
+      </c>
+      <c r="H44" s="47">
+        <v>5.8536585365853657</v>
+      </c>
+      <c r="I44" s="28">
+        <v>16.740119516603848</v>
+      </c>
+      <c r="J44" s="32">
+        <v>5.8761804826862524E-2</v>
+      </c>
+      <c r="K44" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L44" s="11">
+        <v>6.2718677522931074E-2</v>
+      </c>
       <c r="O44" s="13"/>
       <c r="P44" s="13"/>
       <c r="Q44" s="13"/>
@@ -3815,15 +4368,36 @@
       </c>
     </row>
     <row r="45" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C45" s="13"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="28"/>
+      <c r="C45" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="46">
+        <v>17</v>
+      </c>
+      <c r="E45" s="47">
+        <v>6.8292682926829267</v>
+      </c>
+      <c r="F45" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G45" s="47">
+        <v>41.768292682926834</v>
+      </c>
+      <c r="H45" s="47">
+        <v>5.8536585365853657</v>
+      </c>
+      <c r="I45" s="28">
+        <v>16.740119516603848</v>
+      </c>
+      <c r="J45" s="32">
+        <v>5.8761804826862524E-2</v>
+      </c>
+      <c r="K45" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L45" s="11">
+        <v>6.2718677522931074E-2</v>
+      </c>
       <c r="O45" s="13"/>
       <c r="P45" s="13"/>
       <c r="Q45" s="13"/>
@@ -3851,15 +4425,36 @@
       </c>
     </row>
     <row r="46" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C46" s="13"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="28"/>
+      <c r="C46" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="46">
+        <v>18</v>
+      </c>
+      <c r="E46" s="47">
+        <v>4.51219512195122</v>
+      </c>
+      <c r="F46" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G46" s="47">
+        <v>44.969512195121951</v>
+      </c>
+      <c r="H46" s="47">
+        <v>4.6951219512195124</v>
+      </c>
+      <c r="I46" s="28">
+        <v>19.941339028798964</v>
+      </c>
+      <c r="J46" s="32">
+        <v>3.8824763903462747E-2</v>
+      </c>
+      <c r="K46" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L46" s="11">
+        <v>4.3538310891453949E-2</v>
+      </c>
       <c r="O46" s="13"/>
       <c r="P46" s="13"/>
       <c r="Q46" s="13"/>
@@ -3887,15 +4482,36 @@
       </c>
     </row>
     <row r="47" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C47" s="13"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="28"/>
+      <c r="C47" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="46">
+        <v>19</v>
+      </c>
+      <c r="E47" s="47">
+        <v>2.8048780487804876</v>
+      </c>
+      <c r="F47" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G47" s="47">
+        <v>44.969512195121951</v>
+      </c>
+      <c r="H47" s="47">
+        <v>9.3292682926829276</v>
+      </c>
+      <c r="I47" s="28">
+        <v>19.941339028798964</v>
+      </c>
+      <c r="J47" s="32">
+        <v>2.4134312696747106E-2</v>
+      </c>
+      <c r="K47" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L47" s="11">
+        <v>2.8847859684738311E-2</v>
+      </c>
       <c r="O47" s="13"/>
       <c r="P47" s="13"/>
       <c r="Q47" s="13"/>
@@ -3923,15 +4539,36 @@
       </c>
     </row>
     <row r="48" spans="3:34" x14ac:dyDescent="0.2">
-      <c r="C48" s="13"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="28"/>
+      <c r="C48" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="46">
+        <v>20</v>
+      </c>
+      <c r="E48" s="47">
+        <v>2.8353658536585371</v>
+      </c>
+      <c r="F48" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G48" s="47">
+        <v>44.207317073170735</v>
+      </c>
+      <c r="H48" s="47">
+        <v>27.637195121951223</v>
+      </c>
+      <c r="I48" s="28">
+        <v>19.179143906847749</v>
+      </c>
+      <c r="J48" s="32">
+        <v>2.4396642182581321E-2</v>
+      </c>
+      <c r="K48" s="28">
+        <v>15.833163282944582</v>
+      </c>
+      <c r="L48" s="11">
+        <v>2.8930028624876654E-2</v>
+      </c>
       <c r="O48" s="13"/>
       <c r="P48" s="13"/>
       <c r="Q48" s="13"/>

</xml_diff>